<commit_message>
some fix to the standard spreadsheet and align excel2json script to new output path
</commit_message>
<xml_diff>
--- a/Taxonomy_tables_v3.3.xlsx
+++ b/Taxonomy_tables_v3.3.xlsx
@@ -29,6 +29,63 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D4">
+      <text>
+        <t xml:space="preserve">How can we indicate materials that change in height?
+We have cases in which the first floor is MUR and the second floor are metal sheets (INF)
+Options:
+1) We add the attribute MDV: Different materials in in height.
+MDV(MUR,INF)
+2) We modify the description of the MDD to be
+"Different materials in the two directions or in height"
+NOTE: For the LLRS we have LDD and LHV.
+In case we go for option2, the LLRS could be the one indicating the differences (LDD for direction and LHV for heights)
+	-Catalina YepesE
+Any preference?
+@anirudh.rao@globalquakemodel.org
+	-Catalina YepesE</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="D17">
+      <text>
+        <t xml:space="preserve">When and how would we use the NONRES occupancy?  This seems very odd, we do not have NONCOM or other negated occupancy or construction classes, and it is already possible to specify mixed occupancy or other.   Does it make sense to have  a vulnerability curve for a NONRES taxonomy?
+	-Paul Henshaw
+Thank you Paul.
+You are correct that this is not not ideal.
+However, we have in the GRM the case in which the occupancy is explicitly indicated as non residential.
+Do you have any idea?
+The MIX wont work because are not multiple occupancy types.
+Regarding the vulnerability, the taxonomy is not directly applied to the vulnerability. In the cases when NONRES appear, we do a mapping to IND/COM to assign possible vulnerability functions (for the specific case of the GRM)
+	-Catalina YepesE
+So why is this not equivalent to MIX(IND,COM), at least in the context of the GRM?
+	-Paul Henshaw
+Because it's not that the building has mixed used.
+Some of the models include mixed, specially for RES and COM (e.g., first stories commercial and upper floors residential)
+	-Catalina YepesE
+It seems to me that this introduces a concept of uncertainty just for one kind of occupancy: with NONRES meaning "we don't know what occupancy this is but it's not residential"; we do not have any similar language construct for any other element of the taxonomy.   This seems asymmetric.
+	-Paul Henshaw</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="A27">
       <text>
         <t xml:space="preserve">@catalina.yepes@globalquakemodel.org  my proposal is merge material and type together using the same approach used for occupancy:
@@ -42,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="835">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -2205,7 +2262,7 @@
     <t>RSH7</t>
   </si>
   <si>
-    <t xml:space="preserve"> Curved</t>
+    <t>Curved</t>
   </si>
   <si>
     <t>RSH8</t>
@@ -2397,7 +2454,7 @@
     <t>RWO:1</t>
   </si>
   <si>
-    <t>Wooden structurewith light roof covering</t>
+    <t>Wooden structure with light roof covering</t>
   </si>
   <si>
     <t>RWO:2</t>
@@ -2671,7 +2728,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -2711,6 +2768,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2765,7 +2827,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2867,6 +2929,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -4526,11 +4591,11 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="C31:C35"/>
@@ -4600,7 +4665,9 @@
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1"/>
+    <row r="2" ht="13.5" customHeight="1">
+      <c r="D2" s="36"/>
+    </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>45</v>
@@ -5932,7 +5999,7 @@
       <c r="D4" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="37">
         <v>0.0</v>
       </c>
     </row>
@@ -5943,7 +6010,7 @@
       <c r="D5" s="8" t="s">
         <v>671</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="37">
         <v>100.0</v>
       </c>
     </row>
@@ -5954,7 +6021,7 @@
       <c r="D6" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -5965,7 +6032,7 @@
       <c r="D7" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="37">
         <v>300.0</v>
       </c>
     </row>
@@ -5976,7 +6043,7 @@
       <c r="D8" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="37">
         <v>400.0</v>
       </c>
     </row>
@@ -5987,7 +6054,7 @@
       <c r="D9" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="37">
         <v>500.0</v>
       </c>
     </row>
@@ -5995,10 +6062,10 @@
       <c r="C10" s="8" t="s">
         <v>680</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="29" t="s">
         <v>681</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="37">
         <v>600.0</v>
       </c>
     </row>
@@ -6009,7 +6076,7 @@
       <c r="D11" s="8" t="s">
         <v>683</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="37">
         <v>700.0</v>
       </c>
     </row>
@@ -6020,7 +6087,7 @@
       <c r="D12" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="37">
         <v>800.0</v>
       </c>
     </row>
@@ -6031,7 +6098,7 @@
       <c r="D13" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="37">
         <v>900.0</v>
       </c>
     </row>
@@ -6048,7 +6115,7 @@
       <c r="D14" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="37">
         <v>0.0</v>
       </c>
     </row>
@@ -6059,7 +6126,7 @@
       <c r="D15" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="37">
         <v>100.0</v>
       </c>
     </row>
@@ -6070,7 +6137,7 @@
       <c r="D16" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -6081,7 +6148,7 @@
       <c r="D17" s="8" t="s">
         <v>697</v>
       </c>
-      <c r="H17" s="36">
+      <c r="H17" s="37">
         <v>300.0</v>
       </c>
     </row>
@@ -6092,7 +6159,7 @@
       <c r="D18" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="37">
         <v>400.0</v>
       </c>
     </row>
@@ -6103,7 +6170,7 @@
       <c r="D19" s="8" t="s">
         <v>700</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H19" s="37">
         <v>500.0</v>
       </c>
     </row>
@@ -6114,7 +6181,7 @@
       <c r="D20" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="37">
         <v>600.0</v>
       </c>
     </row>
@@ -6125,7 +6192,7 @@
       <c r="D21" s="8" t="s">
         <v>704</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="37">
         <v>700.0</v>
       </c>
     </row>
@@ -6136,7 +6203,7 @@
       <c r="D22" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H22" s="37">
         <v>800.0</v>
       </c>
     </row>
@@ -6147,7 +6214,7 @@
       <c r="D23" s="8" t="s">
         <v>707</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="37">
         <v>900.0</v>
       </c>
     </row>
@@ -6158,7 +6225,7 @@
       <c r="D24" s="8" t="s">
         <v>709</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="37">
         <v>1000.0</v>
       </c>
     </row>
@@ -6169,7 +6236,7 @@
       <c r="D25" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="H25" s="36">
+      <c r="H25" s="37">
         <v>1100.0</v>
       </c>
     </row>
@@ -6180,7 +6247,7 @@
       <c r="D26" s="8" t="s">
         <v>713</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="37">
         <v>1200.0</v>
       </c>
     </row>
@@ -6197,7 +6264,7 @@
       <c r="D27" s="8" t="s">
         <v>634</v>
       </c>
-      <c r="H27" s="36">
+      <c r="H27" s="37">
         <v>0.0</v>
       </c>
       <c r="K27" s="29" t="s">
@@ -6211,7 +6278,7 @@
       <c r="D28" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="H28" s="37">
+      <c r="H28" s="38">
         <v>100.0</v>
       </c>
     </row>
@@ -6222,7 +6289,7 @@
       <c r="D29" s="8" t="s">
         <v>720</v>
       </c>
-      <c r="H29" s="36">
+      <c r="H29" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -6233,7 +6300,7 @@
       <c r="D30" s="8" t="s">
         <v>722</v>
       </c>
-      <c r="H30" s="37">
+      <c r="H30" s="38">
         <v>300.0</v>
       </c>
     </row>
@@ -6244,7 +6311,7 @@
       <c r="D31" s="8" t="s">
         <v>707</v>
       </c>
-      <c r="H31" s="36">
+      <c r="H31" s="37">
         <v>400.0</v>
       </c>
       <c r="K31" s="29" t="s">
@@ -6258,7 +6325,7 @@
       <c r="D32" s="8" t="s">
         <v>725</v>
       </c>
-      <c r="H32" s="37">
+      <c r="H32" s="38">
         <v>500.0</v>
       </c>
     </row>
@@ -6269,7 +6336,7 @@
       <c r="D33" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H33" s="37">
         <v>600.0</v>
       </c>
       <c r="K33" s="29" t="s">
@@ -6283,7 +6350,7 @@
       <c r="D34" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="H34" s="37">
+      <c r="H34" s="38">
         <v>700.0</v>
       </c>
     </row>
@@ -6294,7 +6361,7 @@
       <c r="D35" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H35" s="37">
         <v>800.0</v>
       </c>
     </row>
@@ -6305,7 +6372,7 @@
       <c r="D36" s="8" t="s">
         <v>732</v>
       </c>
-      <c r="H36" s="37">
+      <c r="H36" s="38">
         <v>900.0</v>
       </c>
     </row>
@@ -6316,7 +6383,7 @@
       <c r="D37" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="H37" s="36">
+      <c r="H37" s="37">
         <v>1000.0</v>
       </c>
     </row>
@@ -6327,7 +6394,7 @@
       <c r="D38" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="H38" s="37">
+      <c r="H38" s="38">
         <v>1100.0</v>
       </c>
       <c r="K38" s="29" t="s">
@@ -6341,7 +6408,7 @@
       <c r="D39" s="8" t="s">
         <v>738</v>
       </c>
-      <c r="H39" s="36">
+      <c r="H39" s="37">
         <v>1200.0</v>
       </c>
     </row>
@@ -6352,7 +6419,7 @@
       <c r="D40" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="H40" s="37">
+      <c r="H40" s="38">
         <v>1300.0</v>
       </c>
     </row>
@@ -6363,7 +6430,7 @@
       <c r="D41" s="8" t="s">
         <v>742</v>
       </c>
-      <c r="H41" s="36">
+      <c r="H41" s="37">
         <v>1400.0</v>
       </c>
     </row>
@@ -6374,7 +6441,7 @@
       <c r="D42" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H42" s="37">
+      <c r="H42" s="38">
         <v>1500.0</v>
       </c>
       <c r="K42" s="29" t="s">
@@ -6385,10 +6452,10 @@
       <c r="C43" s="29" t="s">
         <v>744</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="29" t="s">
         <v>745</v>
       </c>
-      <c r="H43" s="36">
+      <c r="H43" s="37">
         <v>1600.0</v>
       </c>
     </row>
@@ -6399,7 +6466,7 @@
       <c r="D44" s="8" t="s">
         <v>747</v>
       </c>
-      <c r="H44" s="37">
+      <c r="H44" s="38">
         <v>1700.0</v>
       </c>
     </row>
@@ -6410,7 +6477,7 @@
       <c r="D45" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="H45" s="36">
+      <c r="H45" s="37">
         <v>1800.0</v>
       </c>
     </row>
@@ -6421,7 +6488,7 @@
       <c r="D46" s="8" t="s">
         <v>751</v>
       </c>
-      <c r="H46" s="37">
+      <c r="H46" s="38">
         <v>1900.0</v>
       </c>
     </row>
@@ -6432,7 +6499,7 @@
       <c r="D47" s="8" t="s">
         <v>753</v>
       </c>
-      <c r="H47" s="36">
+      <c r="H47" s="37">
         <v>2000.0</v>
       </c>
     </row>
@@ -6443,7 +6510,7 @@
       <c r="D48" s="8" t="s">
         <v>755</v>
       </c>
-      <c r="H48" s="37">
+      <c r="H48" s="38">
         <v>2100.0</v>
       </c>
       <c r="K48" s="29" t="s">
@@ -6457,7 +6524,7 @@
       <c r="D49" s="8" t="s">
         <v>757</v>
       </c>
-      <c r="H49" s="36">
+      <c r="H49" s="37">
         <v>2200.0</v>
       </c>
     </row>
@@ -6468,7 +6535,7 @@
       <c r="D50" s="8" t="s">
         <v>759</v>
       </c>
-      <c r="H50" s="37">
+      <c r="H50" s="38">
         <v>2300.0</v>
       </c>
     </row>
@@ -6479,12 +6546,10 @@
       <c r="D51" s="8" t="s">
         <v>761</v>
       </c>
-      <c r="H51" s="36">
+      <c r="H51" s="37">
         <v>2400.0</v>
       </c>
-      <c r="K51" s="29" t="s">
-        <v>372</v>
-      </c>
+      <c r="K51" s="29"/>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
@@ -6499,7 +6564,7 @@
       <c r="D52" s="8" t="s">
         <v>765</v>
       </c>
-      <c r="H52" s="36">
+      <c r="H52" s="38">
         <v>0.0</v>
       </c>
     </row>
@@ -6510,7 +6575,7 @@
       <c r="D53" s="8" t="s">
         <v>767</v>
       </c>
-      <c r="H53" s="36">
+      <c r="H53" s="37">
         <v>100.0</v>
       </c>
     </row>
@@ -6521,7 +6586,7 @@
       <c r="D54" s="8" t="s">
         <v>769</v>
       </c>
-      <c r="H54" s="36">
+      <c r="H54" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -6532,7 +6597,7 @@
       <c r="D55" s="8" t="s">
         <v>771</v>
       </c>
-      <c r="H55" s="36">
+      <c r="H55" s="37">
         <v>300.0</v>
       </c>
     </row>
@@ -7485,13 +7550,13 @@
   <mergeCells count="9">
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B52:B55"/>
-    <mergeCell ref="A27:A51"/>
-    <mergeCell ref="B27:B51"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="A14:A26"/>
     <mergeCell ref="B14:B26"/>
+    <mergeCell ref="A27:A51"/>
+    <mergeCell ref="B27:B51"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -15933,7 +15998,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -50545,7 +50611,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="23.43"/>
     <col customWidth="1" min="2" max="2" width="31.43"/>
-    <col customWidth="1" min="3" max="3" width="11.43"/>
+    <col customWidth="1" min="3" max="3" width="9.29"/>
     <col customWidth="1" min="4" max="4" width="44.43"/>
     <col customWidth="1" min="5" max="5" width="16.29"/>
     <col customWidth="1" min="6" max="6" width="13.71"/>
@@ -52498,7 +52564,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>